<commit_message>
added error checking for watcher and file reader
</commit_message>
<xml_diff>
--- a/JS/1234.xlsx
+++ b/JS/1234.xlsx
@@ -48,6 +48,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Intel 3</t>
     </r>
@@ -57,6 +58,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">rd</t>
     </r>
@@ -65,6 +67,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Generation i5 3470</t>
     </r>
@@ -92,6 +95,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -113,6 +117,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,10 +191,10 @@
   <dimension ref="C1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.37"/>
   </cols>
@@ -222,9 +227,7 @@
       <c r="C4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>200</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">

</xml_diff>